<commit_message>
Agrega nuevos estados de cuenta y actualiza base EC
</commit_message>
<xml_diff>
--- a/Data/Base Junio 2025 Final.xlsx
+++ b/Data/Base Junio 2025 Final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\OneDrive\Escritorio\Escritorio\Vargas Wilches INC\Proyecto, consulta Estados de Cuenta\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6481081D-5210-4566-87AA-CB38E8743486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F7EDBE-FF5C-4CFC-BE10-8F041A63BF7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48E00F1D-9AD1-43FE-9730-2C6D5428D718}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5914" uniqueCount="5914">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5937" uniqueCount="5937">
   <si>
     <t>DOC_EMPRESA</t>
   </si>
@@ -17778,13 +17778,82 @@
   </si>
   <si>
     <t>GRUPO SIDERAS SAS</t>
+  </si>
+  <si>
+    <t>EMIDIO RAFAEL DIAZ CARRETERO</t>
+  </si>
+  <si>
+    <t>CECILIA  CAPELLA DE HERNANDEZ</t>
+  </si>
+  <si>
+    <t>SAIDA RAQUEL BARROSO MEDINA</t>
+  </si>
+  <si>
+    <t>SAMIR  OKE CADAVID</t>
+  </si>
+  <si>
+    <t>RAMON JOSE VIAÑA GONZALEZ</t>
+  </si>
+  <si>
+    <t>EMPRESA SOCIAL DEL ESTADO HOSPITAL LOCAL MARIA LA BAJA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROMOTORA DE DIVERSION S.A. DIVER S.A. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALZATE JIMENEZ &amp; CIA S.A.S </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEXDORAL SAS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLTEXAS JEANS S.A.S </t>
+  </si>
+  <si>
+    <t>AGENCIA DE ADUANAS EAGLE TRADE SAS NIVEL 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GINSA CONSTRUCCIONES S.A.S </t>
+  </si>
+  <si>
+    <t>ISLANDS TOURS S.A.S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAB SAS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LF&amp;F CONSTRUCCIONES SAS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUEVO MILENIO CONSTRUCCIONES SAS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDA COLOMBIA S.A.S </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIVIANOS PESSUTY S.A.S </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LES TROPIQUES SAS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1984 INVERSIONES S.A.S </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INVERSIONES PEREZ ESPINOSA SAS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMARETTO INTERNACIONAL SAS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOLO MOFLES Y LUBRICANTES SAS. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -17796,6 +17865,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -17848,13 +17923,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -18201,10 +18281,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F6EA39-6DA8-4427-A252-3F5866AF73F9}">
-  <dimension ref="A1:B5913"/>
+  <dimension ref="A1:B5936"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" topLeftCell="A5904" workbookViewId="0">
+      <selection activeCell="A5914" sqref="A5914:B5936"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -65517,6 +65597,190 @@
         <v>5913</v>
       </c>
     </row>
+    <row r="5914" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5914" s="7">
+        <v>8538180</v>
+      </c>
+      <c r="B5914" s="7" t="s">
+        <v>5914</v>
+      </c>
+    </row>
+    <row r="5915" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5915" s="7">
+        <v>23170252</v>
+      </c>
+      <c r="B5915" s="7" t="s">
+        <v>5915</v>
+      </c>
+    </row>
+    <row r="5916" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5916" s="5">
+        <v>33193898</v>
+      </c>
+      <c r="B5916" s="6" t="s">
+        <v>5916</v>
+      </c>
+    </row>
+    <row r="5917" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5917" s="7">
+        <v>71638421</v>
+      </c>
+      <c r="B5917" s="7" t="s">
+        <v>5917</v>
+      </c>
+    </row>
+    <row r="5918" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5918" s="6">
+        <v>73095134</v>
+      </c>
+      <c r="B5918" s="6" t="s">
+        <v>5918</v>
+      </c>
+    </row>
+    <row r="5919" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5919" s="7">
+        <v>8060107881</v>
+      </c>
+      <c r="B5919" s="7" t="s">
+        <v>5919</v>
+      </c>
+    </row>
+    <row r="5920" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5920" s="7">
+        <v>8300061229</v>
+      </c>
+      <c r="B5920" s="7" t="s">
+        <v>5920</v>
+      </c>
+    </row>
+    <row r="5921" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5921" s="7">
+        <v>8305121773</v>
+      </c>
+      <c r="B5921" s="7" t="s">
+        <v>5921</v>
+      </c>
+    </row>
+    <row r="5922" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5922" s="7">
+        <v>8600377402</v>
+      </c>
+      <c r="B5922" s="7" t="s">
+        <v>5922</v>
+      </c>
+    </row>
+    <row r="5923" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5923" s="7">
+        <v>9001314246</v>
+      </c>
+      <c r="B5923" s="7" t="s">
+        <v>5923</v>
+      </c>
+    </row>
+    <row r="5924" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5924" s="7">
+        <v>9002204889</v>
+      </c>
+      <c r="B5924" s="7" t="s">
+        <v>5924</v>
+      </c>
+    </row>
+    <row r="5925" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5925" s="7">
+        <v>9008765692</v>
+      </c>
+      <c r="B5925" s="7" t="s">
+        <v>5925</v>
+      </c>
+    </row>
+    <row r="5926" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5926" s="6">
+        <v>9011144452</v>
+      </c>
+      <c r="B5926" s="6" t="s">
+        <v>5926</v>
+      </c>
+    </row>
+    <row r="5927" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5927" s="7">
+        <v>9011460170</v>
+      </c>
+      <c r="B5927" s="7" t="s">
+        <v>5927</v>
+      </c>
+    </row>
+    <row r="5928" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5928" s="7">
+        <v>9011703255</v>
+      </c>
+      <c r="B5928" s="7" t="s">
+        <v>5928</v>
+      </c>
+    </row>
+    <row r="5929" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5929" s="7">
+        <v>9012644258</v>
+      </c>
+      <c r="B5929" s="7" t="s">
+        <v>5929</v>
+      </c>
+    </row>
+    <row r="5930" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5930" s="7">
+        <v>9014156658</v>
+      </c>
+      <c r="B5930" s="7" t="s">
+        <v>5930</v>
+      </c>
+    </row>
+    <row r="5931" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5931" s="7">
+        <v>9014812047</v>
+      </c>
+      <c r="B5931" s="7" t="s">
+        <v>5931</v>
+      </c>
+    </row>
+    <row r="5932" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5932" s="7">
+        <v>9015384950</v>
+      </c>
+      <c r="B5932" s="7" t="s">
+        <v>5932</v>
+      </c>
+    </row>
+    <row r="5933" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5933" s="7">
+        <v>9015926393</v>
+      </c>
+      <c r="B5933" s="7" t="s">
+        <v>5933</v>
+      </c>
+    </row>
+    <row r="5934" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5934" s="7">
+        <v>9016759521</v>
+      </c>
+      <c r="B5934" s="7" t="s">
+        <v>5934</v>
+      </c>
+    </row>
+    <row r="5935" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5935" s="7">
+        <v>9017821904</v>
+      </c>
+      <c r="B5935" s="7" t="s">
+        <v>5935</v>
+      </c>
+    </row>
+    <row r="5936" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5936" s="7">
+        <v>9019097349</v>
+      </c>
+      <c r="B5936" s="7" t="s">
+        <v>5936</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A5913">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>